<commit_message>
Update Sorter Inspection Validation Atlanta.xlsx
</commit_message>
<xml_diff>
--- a/data/Sorter Inspection Validation Atlanta.xlsx
+++ b/data/Sorter Inspection Validation Atlanta.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E203"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,7 +469,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
     <col width="27" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
@@ -5548,6 +5548,31 @@
         </is>
       </c>
       <c r="E203" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>45798</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Strand 7</t>
+        </is>
+      </c>
+      <c r="C204" s="3" t="inlineStr">
+        <is>
+          <t>1:16:09</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E204" s="3" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -5567,7 +5592,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5954,6 +5979,40 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Week Range</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Strands Completed</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>All 8 Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>05-18-25 to 05-24-25</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Strand 7</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">

</xml_diff>